<commit_message>
chore: update example talent template Excel file
</commit_message>
<xml_diff>
--- a/static/files/example_talent_template.xlsx
+++ b/static/files/example_talent_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunakorn.k\Documents\nuxt\asean_talent\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nuxt\new_asean_talent\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED9C34D-71B0-45A1-BD14-AAE70A6E1318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9D8BFA-53F3-4E7B-A7E9-20611BE7F1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62520F6A-1AF7-4942-9BE3-0D0682932D7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{62520F6A-1AF7-4942-9BE3-0D0682932D7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,9 +389,6 @@
     <t>Minneapolis</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>Saliency; Object Detection; Visual Attention</t>
   </si>
   <si>
@@ -567,17 +564,20 @@
   </si>
   <si>
     <t>link_tnrr</t>
+  </si>
+  <si>
+    <t>United States of America</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -586,16 +586,22 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -618,9 +624,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,9 +709,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -742,7 +749,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -848,7 +855,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -990,7 +997,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1000,160 +1007,160 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFA4475-DB17-43E2-BB7F-070024DC0289}">
   <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
-    <col min="4" max="4" width="77.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" customWidth="1"/>
-    <col min="9" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.625" customWidth="1"/>
+    <col min="4" max="4" width="77.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="7" max="7" width="47.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.875" customWidth="1"/>
+    <col min="9" max="10" width="9.875" customWidth="1"/>
+    <col min="11" max="11" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.125" customWidth="1"/>
+    <col min="16" max="16" width="13.375" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="19" width="17.42578125" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" customWidth="1"/>
-    <col min="21" max="21" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" customWidth="1"/>
-    <col min="25" max="25" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.7109375" customWidth="1"/>
-    <col min="27" max="27" width="20.42578125" customWidth="1"/>
-    <col min="28" max="28" width="10.42578125" customWidth="1"/>
-    <col min="29" max="29" width="20.140625" customWidth="1"/>
-    <col min="31" max="31" width="10.85546875" customWidth="1"/>
-    <col min="32" max="32" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.42578125" customWidth="1"/>
-    <col min="34" max="34" width="18.28515625" customWidth="1"/>
-    <col min="35" max="35" width="19.5703125" customWidth="1"/>
+    <col min="18" max="19" width="17.375" customWidth="1"/>
+    <col min="20" max="20" width="18.75" customWidth="1"/>
+    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.25" customWidth="1"/>
+    <col min="25" max="25" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.75" customWidth="1"/>
+    <col min="27" max="27" width="20.375" customWidth="1"/>
+    <col min="28" max="28" width="10.375" customWidth="1"/>
+    <col min="29" max="29" width="20.125" customWidth="1"/>
+    <col min="31" max="31" width="10.875" customWidth="1"/>
+    <col min="32" max="32" width="55.875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.375" customWidth="1"/>
+    <col min="34" max="34" width="18.25" customWidth="1"/>
+    <col min="35" max="35" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75">
+    <row r="1" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>147</v>
-      </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1165,7 +1172,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K2" t="s">
         <v>6</v>
@@ -1243,15 +1250,15 @@
         <v>1759</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -1266,10 +1273,10 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L3" t="s">
         <v>24</v>
@@ -1287,7 +1294,7 @@
         <v>475</v>
       </c>
       <c r="U3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V3" t="s">
         <v>27</v>
@@ -1332,15 +1339,15 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -1355,7 +1362,7 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K4" t="s">
         <v>6</v>
@@ -1433,15 +1440,15 @@
         <v>976</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -1456,7 +1463,7 @@
         <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K5" t="s">
         <v>6</v>
@@ -1534,15 +1541,15 @@
         <v>927</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
@@ -1557,7 +1564,7 @@
         <v>5</v>
       </c>
       <c r="J6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K6" t="s">
         <v>57</v>
@@ -1635,15 +1642,15 @@
         <v>926</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
         <v>69</v>
@@ -1658,7 +1665,7 @@
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K7" t="s">
         <v>72</v>
@@ -1736,15 +1743,15 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
         <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D8" t="s">
         <v>87</v>
@@ -1756,7 +1763,7 @@
         <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K8" t="s">
         <v>89</v>
@@ -1834,15 +1841,15 @@
         <v>871</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D9" t="s">
         <v>101</v>
@@ -1854,7 +1861,7 @@
         <v>5</v>
       </c>
       <c r="J9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K9" t="s">
         <v>72</v>
@@ -1932,15 +1939,15 @@
         <v>858</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
         <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10" t="s">
         <v>114</v>
@@ -1952,52 +1959,52 @@
         <v>5</v>
       </c>
       <c r="J10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L10" t="s">
         <v>116</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="O10" t="s">
         <v>117</v>
       </c>
-      <c r="N10" t="s">
-        <v>117</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>118</v>
-      </c>
-      <c r="P10" t="s">
-        <v>119</v>
       </c>
       <c r="Q10" t="s">
         <v>36</v>
       </c>
       <c r="R10" t="s">
+        <v>119</v>
+      </c>
+      <c r="S10" t="s">
         <v>120</v>
-      </c>
-      <c r="S10" t="s">
-        <v>121</v>
       </c>
       <c r="T10">
         <v>109</v>
       </c>
       <c r="U10" t="s">
+        <v>121</v>
+      </c>
+      <c r="V10" t="s">
         <v>122</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>123</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>124</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>125</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>126</v>
       </c>
       <c r="Z10">
         <v>15</v>
@@ -2018,7 +2025,7 @@
         <v>31</v>
       </c>
       <c r="AF10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AG10">
         <v>42120</v>

</xml_diff>